<commit_message>
add more sample; add comment
</commit_message>
<xml_diff>
--- a/excel/src/main/resources/test.xlsx
+++ b/excel/src/main/resources/test.xlsx
@@ -17,7 +17,8 @@
     <definedName name="quantity">Sheet1!$D$18</definedName>
     <definedName name="remarks">Sheet1!$I$26</definedName>
     <definedName name="row">Sheet1!$A$18:$L$19</definedName>
-    <definedName name="sampleSubmited">Sheet1!$I$24</definedName>
+    <definedName name="sampleSubmitted">Sheet1!$I$24</definedName>
+    <definedName name="title">Sheet1!$B$2</definedName>
     <definedName name="totalAmount">Sheet1!$K$18</definedName>
     <definedName name="unitPrice">Sheet1!$I$18</definedName>
   </definedNames>
@@ -259,11 +260,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -282,6 +286,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -296,27 +321,6 @@
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,7 +602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A13:L29"/>
+  <dimension ref="A2:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -610,257 +614,275 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="18" t="s">
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="19" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19" t="s">
+      <c r="J14" s="15"/>
+      <c r="K14" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L14" s="19"/>
+      <c r="L14" s="15"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="A26:H29"/>
+    <mergeCell ref="I26:L29"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:H21"/>
     <mergeCell ref="I20:L21"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="A24:H25"/>
+    <mergeCell ref="I24:L25"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="B13:C17"/>
     <mergeCell ref="D13:H17"/>
@@ -872,12 +894,6 @@
     <mergeCell ref="D18:H19"/>
     <mergeCell ref="I18:J19"/>
     <mergeCell ref="K18:L19"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="A24:H25"/>
-    <mergeCell ref="I24:L25"/>
-    <mergeCell ref="A26:H29"/>
-    <mergeCell ref="I26:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>